<commit_message>
Cargue de plan de desarrollo Ok
</commit_message>
<xml_diff>
--- a/public/formats/Formato_Plan_Desarrollo.xlsx
+++ b/public/formats/Formato_Plan_Desarrollo.xlsx
@@ -19,10 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
-  <si>
-    <t>COD</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>DIMENSION</t>
   </si>
@@ -37,6 +34,21 @@
   </si>
   <si>
     <t>META</t>
+  </si>
+  <si>
+    <t>COD_D</t>
+  </si>
+  <si>
+    <t>COD_E</t>
+  </si>
+  <si>
+    <t>COD_P</t>
+  </si>
+  <si>
+    <t>COD_S</t>
+  </si>
+  <si>
+    <t>COD_M</t>
   </si>
 </sst>
 </file>
@@ -49,7 +61,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -431,54 +442,54 @@
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="5.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.6640625" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.1640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="5.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.6640625" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26.33203125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="5.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.6640625" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="42.6640625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="5.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.6640625" style="3" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="45.33203125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="5.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.83203125" style="3" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="54" style="2" customWidth="1"/>
     <col min="11" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>